<commit_message>
update2 of excel skills
</commit_message>
<xml_diff>
--- a/skill excel and intro.xlsx
+++ b/skill excel and intro.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Skills</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>apply &amp; variances</t>
+  </si>
+  <si>
+    <t>dataframes treatment</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -632,36 +635,36 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -674,20 +677,22 @@
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
+      <c r="B14" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -699,27 +704,25 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -727,13 +730,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -741,7 +744,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -754,17 +757,23 @@
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>32</v>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -801,6 +810,14 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>